<commit_message>
updated code with single mail for cc'd recipients
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheolmin.hwang\Documents\UiPath\SWMC\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SMWC\github\github\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19410" windowHeight="10410"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -120,12 +120,60 @@
   </si>
   <si>
     <t>SWMC_Client</t>
+  </si>
+  <si>
+    <t>KognivoURL</t>
+  </si>
+  <si>
+    <t>https://0wayqt4bgj.execute-api.us-east-1.amazonaws.com/dev/messages/</t>
+  </si>
+  <si>
+    <t>KognivoKey</t>
+  </si>
+  <si>
+    <t>EmL7DepVBq9RtFSzu2OAN5zIPqCZpspO9TC2y9kV</t>
+  </si>
+  <si>
+    <t>ClientID</t>
+  </si>
+  <si>
+    <t>ClientSecret</t>
+  </si>
+  <si>
+    <t>727481966156-kf0jhl0fu6mthorh6csfdond6eev7mgm.apps.googleusercontent.com</t>
+  </si>
+  <si>
+    <t>MVYZU4SHmYKAZE3PNjYTsoYW</t>
+  </si>
+  <si>
+    <t>outClientID</t>
+  </si>
+  <si>
+    <t>outClientSecret</t>
+  </si>
+  <si>
+    <t>542904632636-b554i9imal6i8auqadqhmn6evdn5ct4v.apps.googleusercontent.com</t>
+  </si>
+  <si>
+    <t>gPGOnDNhcwWsI0HULWamq0br</t>
+  </si>
+  <si>
+    <t>AccessCodeURL_UploadDoc</t>
+  </si>
+  <si>
+    <t>https://staging.reversesoftonline.com/RestServer/session</t>
+  </si>
+  <si>
+    <t>uploadURL_UploadDoc</t>
+  </si>
+  <si>
+    <t>https://staging.reversesoftonline.com/RestServer/image/upload</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -497,16 +545,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -562,7 +610,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -573,34 +621,104 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1579,12 +1697,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.33203125" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1621,7 +1739,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2687,16 +2805,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
-    <col min="3" max="3" width="60.21875" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>